<commit_message>
quyentx added W01 testcase
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="5985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="5985" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
     <sheet name="CreateNewCustomer" sheetId="2" r:id="rId4"/>
     <sheet name="EditCustomer" sheetId="3" r:id="rId5"/>
+    <sheet name="ServiceImporting" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="92">
   <si>
     <t>User</t>
   </si>
@@ -231,16 +232,88 @@
   <si>
     <t>TM04</t>
   </si>
+  <si>
+    <t>W01</t>
+  </si>
+  <si>
+    <t>Date Time</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>LIENLT</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>192.168.0.200</t>
+  </si>
+  <si>
+    <t>ISO 8601</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>123456@a</t>
+  </si>
+  <si>
+    <t>vsii_project.vsii_JIRA_connector</t>
+  </si>
+  <si>
+    <t>collect_project_worklog</t>
+  </si>
+  <si>
+    <t>Service Name</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Webservice Protocol</t>
+  </si>
+  <si>
+    <t>Webservice Host</t>
+  </si>
+  <si>
+    <t>Webservice Port</t>
+  </si>
+  <si>
+    <t>Webservice Path</t>
+  </si>
+  <si>
+    <t>Model Name</t>
+  </si>
+  <si>
+    <t>Decode Method Name</t>
+  </si>
+  <si>
+    <t>TestService3</t>
+  </si>
+  <si>
+    <t>issues.json</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -248,7 +321,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -256,13 +329,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +357,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -376,6 +461,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -439,7 +533,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,10 +565,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -506,7 +599,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -682,23 +774,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -709,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" s="9" t="s">
         <v>16</v>
       </c>
@@ -717,12 +809,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -736,7 +828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
@@ -747,7 +839,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
@@ -758,7 +850,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
@@ -769,7 +861,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>17</v>
@@ -778,7 +870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
@@ -787,7 +879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" s="9" t="s">
         <v>38</v>
       </c>
@@ -798,7 +890,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
@@ -809,7 +901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
@@ -821,26 +913,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="9" t="s">
         <v>67</v>
       </c>
@@ -888,7 +980,7 @@
       </c>
       <c r="P1" s="22"/>
     </row>
-    <row r="2" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="60">
       <c r="A2" s="17"/>
       <c r="B2" s="19">
         <v>1234567</v>
@@ -931,7 +1023,7 @@
       <c r="P2" s="23"/>
       <c r="Q2" s="17"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="P3" s="9" t="s">
         <v>67</v>
       </c>
@@ -944,16 +1036,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="9" t="s">
         <v>64</v>
       </c>
@@ -1003,7 +1095,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="17" customFormat="1" ht="165">
       <c r="B2" s="19"/>
       <c r="C2" s="19" t="s">
         <v>55</v>
@@ -1044,7 +1136,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="Q3" s="9" t="s">
         <v>64</v>
       </c>
@@ -1058,30 +1150,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.75" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.875" customWidth="1"/>
-    <col min="8" max="8" width="22.75" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.25" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.28515625" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1089,18 +1181,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="135">
       <c r="A2" s="15"/>
       <c r="B2" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1135,7 +1227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1167,14 +1259,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="L6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" hidden="1">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
@@ -1182,12 +1274,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1">
       <c r="B13" s="9">
         <v>67743</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1">
       <c r="C14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1202,22 +1294,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="12.375" customWidth="1"/>
-    <col min="7" max="7" width="14.25" customWidth="1"/>
-    <col min="8" max="8" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="14" t="s">
         <v>34</v>
       </c>
@@ -1246,7 +1338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="B2" s="12" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="J3" s="8" t="s">
         <v>34</v>
       </c>
@@ -1283,4 +1375,126 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="2" max="2" width="13.28515625" style="17" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="17"/>
+    <col min="5" max="5" width="12.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="17" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="17"/>
+    <col min="8" max="8" width="11.5703125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="17"/>
+    <col min="10" max="10" width="14.42578125" style="17" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="17"/>
+    <col min="13" max="14" width="12.42578125" style="17" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="45">
+      <c r="A1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60">
+      <c r="B2" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="17">
+        <v>8085</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="O3" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
quyentx: Navigate to create service screen, but still unable to fill data in.
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
   <si>
     <t>User</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t>LIENLT</t>
   </si>
   <si>
     <t>Get</t>
@@ -1379,37 +1376,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17"/>
     <col min="2" max="2" width="13.28515625" style="17" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="17"/>
-    <col min="5" max="5" width="12.42578125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="17" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="17"/>
-    <col min="8" max="8" width="11.5703125" style="17" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="17"/>
-    <col min="10" max="10" width="14.42578125" style="17" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="17"/>
-    <col min="13" max="14" width="12.42578125" style="17" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="17"/>
+    <col min="3" max="3" width="9.140625" style="17"/>
+    <col min="4" max="4" width="12.42578125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="17" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="17"/>
+    <col min="7" max="7" width="11.5703125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="17"/>
+    <col min="9" max="9" width="14.42578125" style="17" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="17"/>
+    <col min="12" max="13" width="12.42578125" style="17" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45">
+    <row r="1" spans="1:14" ht="45">
       <c r="A1" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>0</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>83</v>
@@ -1424,30 +1421,27 @@
         <v>86</v>
       </c>
       <c r="H1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>87</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>11</v>
       </c>
       <c r="M1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="26" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="45">
+      <c r="B2" s="17" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="60">
-      <c r="B2" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>72</v>
@@ -1458,14 +1452,14 @@
       <c r="E2" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="17">
+        <v>8085</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="G2" s="17">
-        <v>8085</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>76</v>
@@ -1473,27 +1467,24 @@
       <c r="J2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="17" t="s">
         <v>79</v>
       </c>
       <c r="M2" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="O3" s="25" t="s">
+    </row>
+    <row r="3" spans="1:14">
+      <c r="N3" s="25" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
quyentx: W01 runs partly OK with Chrome
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -245,9 +245,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Get</t>
-  </si>
-  <si>
     <t>http</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>issues.json</t>
+  </si>
+  <si>
+    <t>8085</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -467,6 +467,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1379,7 +1382,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1403,22 +1406,22 @@
         <v>68</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>85</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>86</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>69</v>
@@ -1433,48 +1436,48 @@
         <v>11</v>
       </c>
       <c r="L1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="26" t="s">
         <v>87</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="45">
       <c r="B2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="17">
+        <v>2</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="17">
-        <v>8085</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="L2" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:14">

</xml_diff>

<commit_message>
QuyenTX: Finished W01 - Implementing W02
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
   <si>
     <t>User</t>
   </si>
@@ -254,9 +254,6 @@
     <t>ISO 8601</t>
   </si>
   <si>
-    <t>basic</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -293,13 +290,22 @@
     <t>Decode Method Name</t>
   </si>
   <si>
-    <t>TestService3</t>
-  </si>
-  <si>
     <t>issues.json</t>
   </si>
   <si>
     <t>8085</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>TestService2</t>
+  </si>
+  <si>
+    <t>TestService1</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -470,6 +476,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1379,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1406,22 +1415,22 @@
         <v>68</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>84</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>85</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>69</v>
@@ -1436,18 +1445,18 @@
         <v>11</v>
       </c>
       <c r="L1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="45">
+    </row>
+    <row r="2" spans="1:14" s="28" customFormat="1" ht="45">
       <c r="B2" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="17">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>72</v>
@@ -1456,38 +1465,77 @@
         <v>73</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="L2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="N3" s="25" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="45">
+      <c r="B3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="N4" s="25" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished W01 test case: added Assert command
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
   <si>
     <t>User</t>
   </si>
@@ -290,9 +290,6 @@
     <t>Decode Method Name</t>
   </si>
   <si>
-    <t>issues.json</t>
-  </si>
-  <si>
     <t>8085</t>
   </si>
   <si>
@@ -302,10 +299,10 @@
     <t>Basic</t>
   </si>
   <si>
-    <t>TestService2</t>
-  </si>
-  <si>
-    <t>TestService1</t>
+    <t>/rest/api/2/search?jql=updated%20%3E%20startOfWeek(-2)%20ORDER%20BY%20updated%20DESC&amp;startAt=0&amp;maxResults=1500&amp;fields=assignee,description,summary,created,updated,duedate,priority,status,worklog,key,id,project,timeestimate,timeoriginalestimate</t>
+  </si>
+  <si>
+    <t>TestService3</t>
   </si>
 </sst>
 </file>
@@ -1388,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1402,7 +1399,7 @@
     <col min="4" max="4" width="12.42578125" style="17" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="17" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="17"/>
-    <col min="7" max="7" width="11.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" style="17" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="17"/>
     <col min="9" max="9" width="14.42578125" style="17" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="17"/>
@@ -1451,12 +1448,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="28" customFormat="1" ht="45">
+    <row r="2" spans="1:14" s="28" customFormat="1" ht="105">
       <c r="B2" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>72</v>
@@ -1465,16 +1462,16 @@
         <v>73</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>75</v>
@@ -1489,53 +1486,14 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="45">
-      <c r="B3" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="N4" s="25" t="s">
+    <row r="3" spans="1:14">
+      <c r="N3" s="25" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
-    <hyperlink ref="K2" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
QuyenTX: Implementing W03 - NullPointerExeption
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="14760" windowHeight="5925" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="14760" windowHeight="5925" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="122">
   <si>
     <t>User</t>
   </si>
@@ -390,12 +390,18 @@
   <si>
     <t>PM11</t>
   </si>
+  <si>
+    <t>W03</t>
+  </si>
+  <si>
+    <t>TestProject</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,7 +427,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +461,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -566,6 +578,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -660,7 +675,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -695,7 +709,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -871,14 +884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -887,7 +900,7 @@
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -898,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="B2" s="9" t="s">
         <v>16</v>
       </c>
@@ -906,12 +919,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -925,7 +938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
@@ -936,7 +949,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
@@ -947,7 +960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
@@ -958,7 +971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>17</v>
@@ -967,7 +980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
@@ -976,7 +989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="B10" s="9" t="s">
         <v>38</v>
       </c>
@@ -987,7 +1000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
@@ -998,7 +1011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1010,14 +1023,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1029,7 +1042,7 @@
     <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="9" t="s">
         <v>67</v>
       </c>
@@ -1077,7 +1090,7 @@
       </c>
       <c r="P1" s="22"/>
     </row>
-    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="60">
       <c r="A2" s="17"/>
       <c r="B2" s="19">
         <v>1234567</v>
@@ -1120,7 +1133,7 @@
       <c r="P2" s="23"/>
       <c r="Q2" s="17"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="P3" s="9" t="s">
         <v>67</v>
       </c>
@@ -1133,16 +1146,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="9" t="s">
         <v>64</v>
       </c>
@@ -1192,7 +1205,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="17" customFormat="1" ht="165">
       <c r="B2" s="19"/>
       <c r="C2" s="19" t="s">
         <v>55</v>
@@ -1233,7 +1246,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="Q3" s="9" t="s">
         <v>64</v>
       </c>
@@ -1247,14 +1260,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
@@ -1270,7 +1283,7 @@
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1278,18 +1291,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="135">
       <c r="A2" s="15"/>
       <c r="B2" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1324,7 +1337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1356,14 +1369,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="L6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
@@ -1371,12 +1384,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1">
       <c r="B13" s="9">
         <v>67743</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1">
       <c r="C14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1391,14 +1404,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
@@ -1406,7 +1419,7 @@
     <col min="9" max="9" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="14" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1448,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" s="12" t="s">
         <v>35</v>
       </c>
@@ -1461,7 +1474,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="J3" s="8" t="s">
         <v>34</v>
       </c>
@@ -1475,14 +1488,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17"/>
     <col min="2" max="2" width="13.28515625" style="17" customWidth="1"/>
@@ -1498,7 +1511,7 @@
     <col min="14" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45">
       <c r="A1" s="25" t="s">
         <v>68</v>
       </c>
@@ -1539,7 +1552,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="28" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="28" customFormat="1" ht="105">
       <c r="B2" s="17" t="s">
         <v>91</v>
       </c>
@@ -1577,9 +1590,27 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="N3" s="25" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="C8" s="25" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1591,14 +1622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
@@ -1613,7 +1644,7 @@
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
@@ -1648,7 +1679,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="B2" s="5" t="s">
         <v>102</v>
       </c>
@@ -1680,12 +1711,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="L3" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>112</v>
       </c>
@@ -1720,7 +1751,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="B5" s="5" t="s">
         <v>113</v>
       </c>
@@ -1752,12 +1783,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="L6" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
@@ -1792,7 +1823,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
         <v>103</v>
@@ -1818,7 +1849,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="L9" s="1" t="s">
         <v>115</v>
       </c>
@@ -1829,14 +1860,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
@@ -1851,7 +1882,7 @@
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
@@ -1886,7 +1917,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="B2" s="5" t="s">
         <v>117</v>
       </c>
@@ -1918,12 +1949,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="L3" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>118</v>
       </c>
@@ -1958,7 +1989,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="B5" s="5" t="s">
         <v>117</v>
       </c>
@@ -1990,12 +2021,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="L6" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>119</v>
       </c>
@@ -2030,7 +2061,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="B8" s="5" t="s">
         <v>117</v>
       </c>
@@ -2062,7 +2093,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="L9" s="1" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
Case W03: implemented, waiting to be verified
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -512,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -561,25 +561,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1492,7 +1489,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1512,104 +1509,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="28" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="28" customFormat="1" ht="105">
-      <c r="B2" s="17" t="s">
+      <c r="N1" s="19"/>
+    </row>
+    <row r="2" spans="1:14" s="24" customFormat="1" ht="105">
+      <c r="A2" s="29"/>
+      <c r="B2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="19" t="s">
         <v>78</v>
       </c>
+      <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="N3" s="25" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="26" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>42</v>
       </c>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19" t="s">
         <v>121</v>
       </c>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="26" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1695,7 +1713,7 @@
       <c r="F2" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="25" t="s">
         <v>107</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -1767,7 +1785,7 @@
       <c r="F5" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="25" t="s">
         <v>107</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -1837,7 +1855,7 @@
       <c r="F8" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="25" t="s">
         <v>107</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1933,7 +1951,7 @@
       <c r="F2" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="25" t="s">
         <v>107</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -2005,7 +2023,7 @@
       <c r="F5" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="25" t="s">
         <v>107</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -2077,7 +2095,7 @@
       <c r="F8" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="25" t="s">
         <v>107</v>
       </c>
       <c r="H8" s="7" t="s">

</xml_diff>

<commit_message>
QuyenTX: Finished W03, verifying W04
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="14760" windowHeight="5925" tabRatio="842"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="14760" windowHeight="5925" tabRatio="842" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="133">
   <si>
     <t>User</t>
   </si>
@@ -395,9 +395,6 @@
     <t>W03</t>
   </si>
   <si>
-    <t>TestProject</t>
-  </si>
-  <si>
     <t>anhptq</t>
   </si>
   <si>
@@ -408,6 +405,30 @@
   </si>
   <si>
     <t>LTS</t>
+  </si>
+  <si>
+    <t>Project Key</t>
+  </si>
+  <si>
+    <t>Selenium Practice</t>
+  </si>
+  <si>
+    <t>SP-1</t>
+  </si>
+  <si>
+    <t>W02</t>
+  </si>
+  <si>
+    <t>Project Department</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>JIRA</t>
+  </si>
+  <si>
+    <t>Project key</t>
   </si>
 </sst>
 </file>
@@ -525,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -590,6 +611,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -897,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1028,7 +1052,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -1039,7 +1063,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="B14" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="9">
         <v>12345678</v>
@@ -1047,7 +1071,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="9">
         <v>12345678</v>
@@ -1055,7 +1079,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" s="9">
         <v>12345678</v>
@@ -1063,7 +1087,7 @@
     </row>
     <row r="17" spans="4:4">
       <c r="D17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1539,17 +1563,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17"/>
     <col min="2" max="2" width="13.28515625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="17"/>
+    <col min="3" max="3" width="13" style="17" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="17" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="17" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="17"/>
@@ -1661,6 +1685,8 @@
         <v>68</v>
       </c>
     </row>
+    <row r="4" spans="1:14" s="30" customFormat="1"/>
+    <row r="5" spans="1:14" s="30" customFormat="1"/>
     <row r="6" spans="1:14">
       <c r="A6" s="26" t="s">
         <v>120</v>
@@ -1668,20 +1694,71 @@
       <c r="B6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="19"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="C6" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:14" ht="30">
       <c r="A7" s="19"/>
       <c r="B7" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="19"/>
+        <v>126</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="26" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30">
+      <c r="A10" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" ht="30">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="26" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1689,6 +1766,7 @@
     <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2187,7 +2265,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2198,7 +2276,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="9">
         <v>12345678</v>
@@ -2206,7 +2284,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="9">
         <v>12345678</v>
@@ -2214,7 +2292,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="9">
         <v>12345678</v>
@@ -2222,7 +2300,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="D5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QuyenTX: Finished W04 - implementing W05
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="136">
   <si>
     <t>User</t>
   </si>
@@ -429,6 +429,15 @@
   </si>
   <si>
     <t>Project key</t>
+  </si>
+  <si>
+    <t>W04</t>
+  </si>
+  <si>
+    <t>Done By</t>
+  </si>
+  <si>
+    <t>Trang-Nguyen Thi Thu Trang</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -614,6 +623,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1563,17 +1575,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17"/>
     <col min="2" max="2" width="13.28515625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="13" style="17" customWidth="1"/>
+    <col min="3" max="3" width="27" style="17" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="17" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="17" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="17"/>
@@ -1759,6 +1771,36 @@
       <c r="E12" s="19"/>
       <c r="F12" s="26" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="19"/>
+      <c r="B16" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="26" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QuyenTX: Implementing W567 - NullPointerException
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="155">
   <si>
     <t>User</t>
   </si>
@@ -438,6 +438,63 @@
   </si>
   <si>
     <t>Trang-Nguyen Thi Thu Trang</t>
+  </si>
+  <si>
+    <t>W05</t>
+  </si>
+  <si>
+    <t>JiraBaseURL</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>time Spent</t>
+  </si>
+  <si>
+    <t>start time</t>
+  </si>
+  <si>
+    <t>http://192.168.0.200:8085/secure/Dashboard.jspa</t>
+  </si>
+  <si>
+    <t>trangntt</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>ERPusername</t>
+  </si>
+  <si>
+    <t>ERPpassword</t>
+  </si>
+  <si>
+    <t>02:00</t>
+  </si>
+  <si>
+    <t>Lien-Le Thi Lien</t>
+  </si>
+  <si>
+    <t>timeSpentOnERP</t>
+  </si>
+  <si>
+    <t>doneByOnERP</t>
+  </si>
+  <si>
+    <t>W06</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>W07</t>
   </si>
 </sst>
 </file>
@@ -470,7 +527,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,6 +567,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,7 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -626,6 +689,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1575,10 +1650,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1588,11 +1663,12 @@
     <col min="3" max="3" width="27" style="17" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="17" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="17"/>
-    <col min="7" max="7" width="43.42578125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="17"/>
-    <col min="9" max="9" width="14.42578125" style="17" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="17"/>
+    <col min="6" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="17"/>
     <col min="12" max="13" width="12.42578125" style="17" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="17"/>
   </cols>
@@ -1747,7 +1823,7 @@
       </c>
       <c r="F10" s="19"/>
     </row>
-    <row r="11" spans="1:14" ht="30">
+    <row r="11" spans="1:14">
       <c r="A11" s="19"/>
       <c r="B11" s="19" t="s">
         <v>130</v>
@@ -1795,12 +1871,198 @@
       </c>
       <c r="D16" s="19"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:11">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="26" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60">
+      <c r="B21" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="33">
+        <v>42455.683333333334</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="K22" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30">
+      <c r="A25" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="I25" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60">
+      <c r="B26" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="J27" s="35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30">
+      <c r="A30" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="60">
+      <c r="B31" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G31" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="J32" s="35" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QuyenTX: Finished W05, editing W06,07
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="154">
   <si>
     <t>User</t>
   </si>
@@ -467,9 +467,6 @@
     <t>12345678</t>
   </si>
   <si>
-    <t>4h</t>
-  </si>
-  <si>
     <t>ERPusername</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>02:00</t>
   </si>
   <si>
-    <t>Lien-Le Thi Lien</t>
-  </si>
-  <si>
     <t>timeSpentOnERP</t>
   </si>
   <si>
@@ -495,6 +489,9 @@
   </si>
   <si>
     <t>W07</t>
+  </si>
+  <si>
+    <t>LIENLT</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1650,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1715,7 +1712,7 @@
       </c>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" s="24" customFormat="1" ht="105">
+    <row r="2" spans="1:14" s="24" customFormat="1" ht="195">
       <c r="A2" s="29"/>
       <c r="B2" s="19" t="s">
         <v>91</v>
@@ -1899,16 +1896,16 @@
         <v>141</v>
       </c>
       <c r="G20" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="H20" s="34" t="s">
-        <v>147</v>
-      </c>
       <c r="I20" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60">
@@ -1922,7 +1919,7 @@
         <v>144</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F21" s="33">
         <v>42455.683333333334</v>
@@ -1934,10 +1931,10 @@
         <v>144</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1947,7 +1944,7 @@
     </row>
     <row r="25" spans="1:11" ht="30">
       <c r="A25" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B25" s="34" t="s">
         <v>137</v>
@@ -1962,16 +1959,16 @@
         <v>140</v>
       </c>
       <c r="F25" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="G25" s="34" t="s">
-        <v>147</v>
-      </c>
       <c r="H25" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I25" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60">
@@ -1985,7 +1982,7 @@
         <v>144</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F26" s="33" t="s">
         <v>122</v>
@@ -1994,7 +1991,7 @@
         <v>144</v>
       </c>
       <c r="H26" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I26" s="19" t="s">
         <v>135</v>
@@ -2002,12 +1999,12 @@
     </row>
     <row r="27" spans="1:11">
       <c r="J27" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30">
       <c r="A30" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>137</v>
@@ -2022,16 +2019,16 @@
         <v>140</v>
       </c>
       <c r="F30" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="34" t="s">
-        <v>147</v>
-      </c>
       <c r="H30" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I30" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60">
@@ -2045,7 +2042,7 @@
         <v>144</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F31" s="33" t="s">
         <v>122</v>
@@ -2054,15 +2051,15 @@
         <v>144</v>
       </c>
       <c r="H31" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="J32" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QuyenTX: 2 cases runs successfully with new scenario(create new projects in both JIRA and OpenERP)
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="175">
   <si>
     <t>User</t>
   </si>
@@ -492,6 +492,69 @@
   </si>
   <si>
     <t>timeSpentERp</t>
+  </si>
+  <si>
+    <t>projectListXpath</t>
+  </si>
+  <si>
+    <t>issueListXpath</t>
+  </si>
+  <si>
+    <t>worklogListXpath</t>
+  </si>
+  <si>
+    <t>firstProjectXpath</t>
+  </si>
+  <si>
+    <t>firstWorklogXpath</t>
+  </si>
+  <si>
+    <t>html/body/div/section/div/div/section/div[1]/div[2]/div/table/tbody</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div[2]/div/section/div/div/div/div/div/div/div[1]/div[1]/div/div[1]/div[2]/div/ol</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div[2]/div/section/div/div/div/div/div/div/div[2]/div[1]/div/div/div/div[1]/div[5]/div[2]/div[2]/div[2]</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div/div/section/div[1]/div[2]/div/table/tbody/tr[1]/td[2]/a</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div[2]/div/section/div/div/div/div/div/div/div[1]/div[1]/div/div[1]/div[2]/div/ol/li["+issueListSize+"]/a/span[2]</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div[2]/div/section/div/div/div/div/div/div/div[2]/div[1]/div/div/div/div[1]/div[5]/div[2]/div[2]/div[2]/div["+worklogListSize+"]</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div[2]/div/section/div/div/div/div/div/div/div[2]/div[1]/div/div/div/div[1]/div[5]/div[2]/div[2]/div[2]/div["+worklogListSize+"]/div/div[2]/a</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div[2]/div/section/div/div/div/div/div/div/div[2]/div[1]/div/div/div/div[1]/div[5]/div[2]/div[2]/div[2]/div["+worklogListSize+"]/div/div[3]/ul/li/dl[1]/dd</t>
+  </si>
+  <si>
+    <t>firstWorklogNameXpath</t>
+  </si>
+  <si>
+    <t>firstWorklogTimeXpath</t>
+  </si>
+  <si>
+    <t>CheckJIRA</t>
+  </si>
+  <si>
+    <t>html/body/div/section/div/div/section/div[1]/div[2]/div/table/tbody/tr[1]/td[3]</t>
+  </si>
+  <si>
+    <t>firstProjectKeyXpath</t>
+  </si>
+  <si>
+    <t>firstIssueNameXpath</t>
+  </si>
+  <si>
+    <t>firstIssueKeyXpath</t>
+  </si>
+  <si>
+    <t>html/body/div[1]/section/div[2]/div/section/div/div/div/div/div/div/div[1]/div[1]/div/div[1]/div[2]/div/ol/li["+issueListSize+"]/a/span[1]</t>
   </si>
 </sst>
 </file>
@@ -615,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -701,6 +764,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1650,25 +1716,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="17" customWidth="1"/>
     <col min="3" max="3" width="27" style="17" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="17" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" style="17" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="17" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="17" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="17"/>
+    <col min="8" max="8" width="24.5703125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" style="17" customWidth="1"/>
     <col min="12" max="13" width="12.42578125" style="17" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="17"/>
   </cols>
@@ -2044,15 +2110,100 @@
         <v>150</v>
       </c>
     </row>
+    <row r="34" spans="1:14" ht="30">
+      <c r="A34" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="H34" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="I34" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="J34" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="K34" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="L34" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="M34" s="33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="225">
+      <c r="B35" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="I35" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="30">
+      <c r="N36" s="34" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
     <hyperlink ref="B21" r:id="rId2"/>
     <hyperlink ref="B26" r:id="rId3"/>
     <hyperlink ref="B31" r:id="rId4"/>
+    <hyperlink ref="C35" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>